<commit_message>
feat: new tables, template update
</commit_message>
<xml_diff>
--- a/printer/templates/template_0.xlsx
+++ b/printer/templates/template_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\#### D\Work\# python\chickenPrinter\printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A8B4E9-EE1D-46A8-AE19-B8AC70EF819F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E06153-56D6-45E7-BE56-87906305A988}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -88,70 +88,25 @@
     <t>user</t>
   </si>
   <si>
-    <t>wryeryerty ert ety 34563 456</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 457</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 458</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 459</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 460</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 461</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 462</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 463</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 464</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 465</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 466</t>
-  </si>
-  <si>
-    <t>wryeryerty ert ety 34563 467</t>
-  </si>
-  <si>
-    <t>Arial</t>
+    <t>Bahnschrift Light Condensed</t>
+  </si>
+  <si>
+    <t>Схавай ещё этих булок</t>
+  </si>
+  <si>
+    <t>Bahnschrift SemiLight Condensed</t>
+  </si>
+  <si>
+    <t>Bahnschrift Condensed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="5"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="4"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -164,52 +119,92 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="3"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="4"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="5"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="3"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <name val="Arial"/>
+      <name val="Bahnschrift Light Condensed"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Bahnschrift Light Condensed"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
+      <name val="Bahnschrift Light Condensed"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="13"/>
-      <name val="Arial"/>
+      <name val="Bahnschrift Light Condensed"/>
       <family val="2"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Bahnschrift Light Condensed"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Condens Bold"/>
     </font>
   </fonts>
   <fills count="2">
@@ -392,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -429,32 +424,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -772,13 +790,16 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="2.5703125" customWidth="1"/>
+    <col min="1" max="1" width="0.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="13" max="13" width="1.28515625" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" customWidth="1"/>
+    <col min="15" max="15" width="1.7109375" customWidth="1"/>
     <col min="1024" max="1025" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -838,341 +859,349 @@
     </row>
     <row r="4" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="28">
+      <c r="B4" s="51">
         <v>3</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="14"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="54"/>
     </row>
     <row r="5" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="24">
+      <c r="B5" s="50">
         <v>4</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="14"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="54"/>
     </row>
     <row r="6" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="24">
+      <c r="B6" s="49">
         <v>5</v>
       </c>
-      <c r="C6" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="14"/>
+      <c r="C6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="24">
+      <c r="B7" s="48">
         <v>6</v>
       </c>
-      <c r="C7" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="14"/>
+      <c r="C7" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="54"/>
     </row>
     <row r="8" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="24">
+      <c r="B8" s="47">
         <v>7</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="14"/>
+      <c r="C8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="54"/>
     </row>
     <row r="9" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="24">
+      <c r="B9" s="28">
         <v>8</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="14"/>
+      <c r="C9" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="54"/>
     </row>
     <row r="10" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="24">
+      <c r="B10" s="46">
         <v>9</v>
       </c>
-      <c r="C10" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="14"/>
+      <c r="C10" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="54"/>
     </row>
     <row r="11" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="24">
+      <c r="B11" s="45">
         <v>10</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="14"/>
+      <c r="C11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="54"/>
     </row>
     <row r="12" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="24">
+      <c r="B12" s="44">
         <v>11</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="14"/>
+      <c r="C12" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="54"/>
     </row>
     <row r="13" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="24">
+      <c r="B13" s="43">
         <v>12</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="14"/>
-    </row>
-    <row r="14" spans="1:15" ht="14.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="54"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="24">
+      <c r="B14" s="42">
         <v>13</v>
       </c>
-      <c r="C14" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="14"/>
-    </row>
-    <row r="15" spans="1:15" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="54"/>
+    </row>
+    <row r="15" spans="1:15" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="24">
+      <c r="B15" s="41">
         <v>14</v>
       </c>
-      <c r="C15" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="14"/>
-    </row>
-    <row r="16" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="54"/>
+    </row>
+    <row r="16" spans="1:15" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="14"/>
-    </row>
-    <row r="17" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="59">
+        <v>15</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="54"/>
+    </row>
+    <row r="17" spans="1:15" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="14"/>
-    </row>
-    <row r="18" spans="1:15" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="60">
+        <v>16</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="54"/>
+    </row>
+    <row r="18" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="27"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="55"/>
+      <c r="M18" s="55"/>
+      <c r="N18" s="56"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="27"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="24"/>
       <c r="O19" s="14"/>
     </row>
-    <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="27"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="24"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="1:15" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>